<commit_message>
preapre: proses import batch data siswa
</commit_message>
<xml_diff>
--- a/writable/uploads/template/form_import_siswa.xlsx
+++ b/writable/uploads/template/form_import_siswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Reza\php\spmb\writable\uploads\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F22E840F-C5E8-48CC-A480-76118E7D8310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D98B408-E2D1-4468-BDDC-64B46933E001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{472507E7-C6A7-43FA-B6DD-67503586CBC9}"/>
   </bookViews>
@@ -36,26 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>NIP</t>
   </si>
   <si>
-    <t>NPSN</t>
-  </si>
-  <si>
-    <t>Nama Sekolah</t>
-  </si>
-  <si>
     <t>Alamat</t>
   </si>
   <si>
-    <t>Alamat Sekolah</t>
-  </si>
-  <si>
-    <t>Status (Swasta/Negeri)</t>
-  </si>
-  <si>
     <t>No. KK</t>
   </si>
   <si>
@@ -74,16 +62,10 @@
     <t>Tanggal Lahir</t>
   </si>
   <si>
-    <t>Jenis Kelamin</t>
-  </si>
-  <si>
     <t>Status (WNI/WNA)</t>
   </si>
   <si>
-    <t>Kabupaten Asal Sekolah</t>
-  </si>
-  <si>
-    <t>Kecamatan Asal Sekolah</t>
+    <t>Jenis Kelamin (L/P)</t>
   </si>
 </sst>
 </file>
@@ -488,77 +470,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A307ED07-8750-43E4-8BE0-DDC4B066E979}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -569,14 +528,8 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -587,14 +540,8 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -605,14 +552,8 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -623,14 +564,8 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -641,14 +576,8 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -659,14 +588,8 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -677,14 +600,8 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -695,14 +612,8 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -713,14 +624,8 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -731,12 +636,6 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update: format text file
</commit_message>
<xml_diff>
--- a/writable/uploads/template/form_import_siswa.xlsx
+++ b/writable/uploads/template/form_import_siswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Reza\php\spmb\writable\uploads\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D98B408-E2D1-4468-BDDC-64B46933E001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF4AF5E-92C6-462C-8977-3E45621579AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{472507E7-C6A7-43FA-B6DD-67503586CBC9}"/>
   </bookViews>
@@ -129,12 +129,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -473,11 +475,12 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="4" width="9.140625" style="4"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -518,10 +521,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -530,10 +533,10 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -542,10 +545,10 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -554,10 +557,10 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -566,10 +569,10 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -578,10 +581,10 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -590,10 +593,10 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -602,10 +605,10 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -614,10 +617,10 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -626,10 +629,10 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>

</xml_diff>

<commit_message>
fix: tambahkan binding tambahan siswa dan perbaikan view
</commit_message>
<xml_diff>
--- a/writable/uploads/template/form_import_siswa.xlsx
+++ b/writable/uploads/template/form_import_siswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Reza\php\spmb\writable\uploads\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF4AF5E-92C6-462C-8977-3E45621579AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29C2F6D-9B97-4C0A-854C-85D8EC10EBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{472507E7-C6A7-43FA-B6DD-67503586CBC9}"/>
   </bookViews>
@@ -36,23 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>NIP</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Alamat</t>
   </si>
   <si>
-    <t>No. KK</t>
-  </si>
-  <si>
-    <t>No. PKH</t>
-  </si>
-  <si>
-    <t>No. PIP</t>
-  </si>
-  <si>
     <t>Nama Siswa</t>
   </si>
   <si>
@@ -66,6 +54,33 @@
   </si>
   <si>
     <t>Jenis Kelamin (L/P)</t>
+  </si>
+  <si>
+    <t>NISN</t>
+  </si>
+  <si>
+    <t>NIK</t>
+  </si>
+  <si>
+    <t>Nama Ibu Kandung</t>
+  </si>
+  <si>
+    <t>Desa</t>
+  </si>
+  <si>
+    <t>Kabupaten</t>
+  </si>
+  <si>
+    <t>Kecamatan</t>
+  </si>
+  <si>
+    <t>Nomor KK</t>
+  </si>
+  <si>
+    <t>Nomor PKH</t>
+  </si>
+  <si>
+    <t>Nomor PIP</t>
   </si>
 </sst>
 </file>
@@ -472,173 +487,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A307ED07-8750-43E4-8BE0-DDC4B066E979}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="4"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="1"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>